<commit_message>
Added exclude items list
</commit_message>
<xml_diff>
--- a/Requirements/TotalItemList.xlsx
+++ b/Requirements/TotalItemList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saina\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Source\InventoryControl\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -676,12 +676,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -807,7 +813,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -819,6 +825,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1327,7 +1334,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F225"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
+      <selection activeCell="C214" sqref="C214"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4083,11 +4092,11 @@
         <v>195</v>
       </c>
       <c r="B196" s="5"/>
-      <c r="C196" s="5" t="s">
+      <c r="C196" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="D196" s="5"/>
-      <c r="E196" s="5" t="s">
+      <c r="D196" s="11"/>
+      <c r="E196" s="11" t="s">
         <v>193</v>
       </c>
       <c r="F196" s="6"/>
@@ -4097,11 +4106,11 @@
         <v>196</v>
       </c>
       <c r="B197" s="5"/>
-      <c r="C197" s="5" t="s">
+      <c r="C197" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="D197" s="5"/>
-      <c r="E197" s="5" t="s">
+      <c r="D197" s="11"/>
+      <c r="E197" s="11" t="s">
         <v>193</v>
       </c>
       <c r="F197" s="6"/>
@@ -4319,11 +4328,11 @@
         <v>211</v>
       </c>
       <c r="B213" s="5"/>
-      <c r="C213" s="5" t="s">
+      <c r="C213" s="11" t="s">
         <v>190</v>
       </c>
-      <c r="D213" s="5"/>
-      <c r="E213" s="5" t="s">
+      <c r="D213" s="11"/>
+      <c r="E213" s="11" t="s">
         <v>193</v>
       </c>
       <c r="F213" s="6"/>

</xml_diff>

<commit_message>
ADDED PROCESSING SLIPPAGE AND ITS FUNCTIONALITY
</commit_message>
<xml_diff>
--- a/Requirements/TotalItemList.xlsx
+++ b/Requirements/TotalItemList.xlsx
@@ -813,7 +813,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -826,6 +826,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1334,8 +1335,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F225"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A191" workbookViewId="0">
-      <selection activeCell="C214" sqref="C214"/>
+    <sheetView tabSelected="1" topLeftCell="A199" workbookViewId="0">
+      <selection activeCell="D219" sqref="D219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4342,11 +4343,11 @@
         <v>212</v>
       </c>
       <c r="B214" s="5"/>
-      <c r="C214" t="s">
+      <c r="C214" s="12" t="s">
         <v>188</v>
       </c>
-      <c r="D214" s="5"/>
-      <c r="E214" s="5" t="s">
+      <c r="D214" s="11"/>
+      <c r="E214" s="11" t="s">
         <v>193</v>
       </c>
       <c r="F214" s="6"/>
@@ -4482,11 +4483,11 @@
         <v>222</v>
       </c>
       <c r="B224" s="5"/>
-      <c r="C224" s="5" t="s">
+      <c r="C224" s="11" t="s">
         <v>203</v>
       </c>
-      <c r="D224" s="5"/>
-      <c r="E224" s="5" t="s">
+      <c r="D224" s="11"/>
+      <c r="E224" s="11" t="s">
         <v>193</v>
       </c>
       <c r="F224" s="6"/>

</xml_diff>

<commit_message>
Changes for branch combobox
Changes for branch combobox
</commit_message>
<xml_diff>
--- a/Requirements/TotalItemList.xlsx
+++ b/Requirements/TotalItemList.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Source\InventoryControl\Requirements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\InventoryControl\Requirements\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -813,7 +813,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -822,12 +822,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1024,7 +1025,13 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:F225" totalsRowShown="0" headerRowDxfId="9" headerRowBorderDxfId="8" tableBorderDxfId="7" totalsRowBorderDxfId="6">
-  <autoFilter ref="A1:F225"/>
+  <autoFilter ref="A1:F225">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Pending"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <tableColumns count="6">
     <tableColumn id="1" name="S No" dataDxfId="5"/>
     <tableColumn id="2" name="Area" dataDxfId="4"/>
@@ -1337,7 +1344,7 @@
   <dimension ref="A1:F225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F215" sqref="F215"/>
+      <selection activeCell="D185" sqref="D185"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1369,7 +1376,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -1385,7 +1392,7 @@
       </c>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -1399,7 +1406,7 @@
       </c>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -1413,7 +1420,7 @@
       </c>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -1427,7 +1434,7 @@
       </c>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -1441,7 +1448,7 @@
       </c>
       <c r="F6" s="6"/>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -1455,7 +1462,7 @@
       </c>
       <c r="F7" s="6"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -1469,7 +1476,7 @@
       </c>
       <c r="F8" s="6"/>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -1483,7 +1490,7 @@
       </c>
       <c r="F9" s="6"/>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1497,7 +1504,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1511,7 +1518,7 @@
       </c>
       <c r="F11" s="6"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1525,7 +1532,7 @@
       </c>
       <c r="F12" s="6"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1539,7 +1546,7 @@
       </c>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1553,7 +1560,7 @@
       </c>
       <c r="F14" s="6"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1567,7 +1574,7 @@
       </c>
       <c r="F15" s="6"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1581,7 +1588,7 @@
       </c>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1595,7 +1602,7 @@
       </c>
       <c r="F17" s="6"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1609,7 +1616,7 @@
       </c>
       <c r="F18" s="6"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1623,7 +1630,7 @@
       </c>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1637,7 +1644,7 @@
       </c>
       <c r="F20" s="6"/>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1651,7 +1658,7 @@
       </c>
       <c r="F21" s="6"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1665,7 +1672,7 @@
       </c>
       <c r="F22" s="6"/>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1679,7 +1686,7 @@
       </c>
       <c r="F23" s="6"/>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1693,7 +1700,7 @@
       </c>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -1707,7 +1714,7 @@
       </c>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1721,7 +1728,7 @@
       </c>
       <c r="F26" s="6"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -1735,7 +1742,7 @@
       </c>
       <c r="F27" s="6"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -1749,7 +1756,7 @@
       </c>
       <c r="F28" s="6"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -1763,7 +1770,7 @@
       </c>
       <c r="F29" s="6"/>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -1777,7 +1784,7 @@
       </c>
       <c r="F30" s="6"/>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -1791,7 +1798,7 @@
       </c>
       <c r="F31" s="6"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -1815,11 +1822,11 @@
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F33" s="6"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -1833,7 +1840,7 @@
       </c>
       <c r="F34" s="6"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -1847,7 +1854,7 @@
       </c>
       <c r="F35" s="6"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -1861,7 +1868,7 @@
       </c>
       <c r="F36" s="6"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -1889,7 +1896,7 @@
       </c>
       <c r="F38" s="6"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -1903,7 +1910,7 @@
       </c>
       <c r="F39" s="6"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -1917,7 +1924,7 @@
       </c>
       <c r="F40" s="6"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -1931,7 +1938,7 @@
       </c>
       <c r="F41" s="6"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -1945,7 +1952,7 @@
       </c>
       <c r="F42" s="6"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -1959,7 +1966,7 @@
       </c>
       <c r="F43" s="6"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -1973,7 +1980,7 @@
       </c>
       <c r="F44" s="6"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -1987,7 +1994,7 @@
       </c>
       <c r="F45" s="6"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -2001,7 +2008,7 @@
       </c>
       <c r="F46" s="6"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -2015,7 +2022,7 @@
       </c>
       <c r="F47" s="6"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -2029,7 +2036,7 @@
       </c>
       <c r="F48" s="6"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -2043,7 +2050,7 @@
       </c>
       <c r="F49" s="6"/>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -2057,7 +2064,7 @@
       </c>
       <c r="F50" s="6"/>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -2071,7 +2078,7 @@
       </c>
       <c r="F51" s="6"/>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4">
         <v>51</v>
       </c>
@@ -2085,7 +2092,7 @@
       </c>
       <c r="F52" s="6"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>52</v>
       </c>
@@ -2099,7 +2106,7 @@
       </c>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>53</v>
       </c>
@@ -2113,7 +2120,7 @@
       </c>
       <c r="F54" s="6"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A55" s="4">
         <v>54</v>
       </c>
@@ -2127,7 +2134,7 @@
       </c>
       <c r="F55" s="6"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A56" s="4">
         <v>55</v>
       </c>
@@ -2141,7 +2148,7 @@
       </c>
       <c r="F56" s="6"/>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4">
         <v>56</v>
       </c>
@@ -2155,7 +2162,7 @@
       </c>
       <c r="F57" s="6"/>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A58" s="4">
         <v>57</v>
       </c>
@@ -2169,7 +2176,7 @@
       </c>
       <c r="F58" s="6"/>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A59" s="4">
         <v>58</v>
       </c>
@@ -2183,7 +2190,7 @@
       </c>
       <c r="F59" s="6"/>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A60" s="4">
         <v>59</v>
       </c>
@@ -2197,7 +2204,7 @@
       </c>
       <c r="F60" s="6"/>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A61" s="4">
         <v>60</v>
       </c>
@@ -2211,7 +2218,7 @@
       </c>
       <c r="F61" s="6"/>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A62" s="4">
         <v>61</v>
       </c>
@@ -2225,7 +2232,7 @@
       </c>
       <c r="F62" s="6"/>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4">
         <v>62</v>
       </c>
@@ -2239,7 +2246,7 @@
       </c>
       <c r="F63" s="6"/>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A64" s="4">
         <v>63</v>
       </c>
@@ -2253,7 +2260,7 @@
       </c>
       <c r="F64" s="6"/>
     </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A65" s="4">
         <v>64</v>
       </c>
@@ -2267,7 +2274,7 @@
       </c>
       <c r="F65" s="6"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A66" s="4">
         <v>65</v>
       </c>
@@ -2281,7 +2288,7 @@
       </c>
       <c r="F66" s="6"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A67" s="4">
         <v>66</v>
       </c>
@@ -2295,7 +2302,7 @@
       </c>
       <c r="F67" s="6"/>
     </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A68" s="4">
         <v>67</v>
       </c>
@@ -2309,7 +2316,7 @@
       </c>
       <c r="F68" s="6"/>
     </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4">
         <v>68</v>
       </c>
@@ -2323,7 +2330,7 @@
       </c>
       <c r="F69" s="6"/>
     </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A70" s="4">
         <v>69</v>
       </c>
@@ -2337,7 +2344,7 @@
       </c>
       <c r="F70" s="6"/>
     </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A71" s="4">
         <v>70</v>
       </c>
@@ -2351,7 +2358,7 @@
       </c>
       <c r="F71" s="6"/>
     </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A72" s="4">
         <v>71</v>
       </c>
@@ -2365,7 +2372,7 @@
       </c>
       <c r="F72" s="6"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A73" s="4">
         <v>72</v>
       </c>
@@ -2379,7 +2386,7 @@
       </c>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A74" s="4">
         <v>73</v>
       </c>
@@ -2393,7 +2400,7 @@
       </c>
       <c r="F74" s="6"/>
     </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A75" s="4">
         <v>74</v>
       </c>
@@ -2407,7 +2414,7 @@
       </c>
       <c r="F75" s="6"/>
     </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A76" s="4">
         <v>75</v>
       </c>
@@ -2421,7 +2428,7 @@
       </c>
       <c r="F76" s="6"/>
     </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A77" s="4">
         <v>76</v>
       </c>
@@ -2435,7 +2442,7 @@
       </c>
       <c r="F77" s="6"/>
     </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A78" s="4">
         <v>77</v>
       </c>
@@ -2449,7 +2456,7 @@
       </c>
       <c r="F78" s="6"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A79" s="4">
         <v>78</v>
       </c>
@@ -2463,7 +2470,7 @@
       </c>
       <c r="F79" s="6"/>
     </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A80" s="4">
         <v>79</v>
       </c>
@@ -2477,7 +2484,7 @@
       </c>
       <c r="F80" s="6"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A81" s="4">
         <v>80</v>
       </c>
@@ -2491,7 +2498,7 @@
       </c>
       <c r="F81" s="6"/>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A82" s="4">
         <v>81</v>
       </c>
@@ -2505,7 +2512,7 @@
       </c>
       <c r="F82" s="6"/>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A83" s="4">
         <v>82</v>
       </c>
@@ -2519,7 +2526,7 @@
       </c>
       <c r="F83" s="6"/>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A84" s="4">
         <v>83</v>
       </c>
@@ -2533,7 +2540,7 @@
       </c>
       <c r="F84" s="6"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A85" s="4">
         <v>84</v>
       </c>
@@ -2547,7 +2554,7 @@
       </c>
       <c r="F85" s="6"/>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A86" s="4">
         <v>85</v>
       </c>
@@ -2561,7 +2568,7 @@
       </c>
       <c r="F86" s="6"/>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A87" s="4">
         <v>86</v>
       </c>
@@ -2575,7 +2582,7 @@
       </c>
       <c r="F87" s="6"/>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A88" s="4">
         <v>87</v>
       </c>
@@ -2589,7 +2596,7 @@
       </c>
       <c r="F88" s="6"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A89" s="4">
         <v>88</v>
       </c>
@@ -2603,7 +2610,7 @@
       </c>
       <c r="F89" s="6"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A90" s="4">
         <v>89</v>
       </c>
@@ -2617,7 +2624,7 @@
       </c>
       <c r="F90" s="6"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A91" s="4">
         <v>90</v>
       </c>
@@ -2631,7 +2638,7 @@
       </c>
       <c r="F91" s="6"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A92" s="4">
         <v>91</v>
       </c>
@@ -2645,7 +2652,7 @@
       </c>
       <c r="F92" s="6"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A93" s="4">
         <v>92</v>
       </c>
@@ -2659,7 +2666,7 @@
       </c>
       <c r="F93" s="6"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A94" s="4">
         <v>93</v>
       </c>
@@ -2673,7 +2680,7 @@
       </c>
       <c r="F94" s="6"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A95" s="4">
         <v>94</v>
       </c>
@@ -2687,7 +2694,7 @@
       </c>
       <c r="F95" s="6"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A96" s="4">
         <v>95</v>
       </c>
@@ -2701,7 +2708,7 @@
       </c>
       <c r="F96" s="6"/>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A97" s="4">
         <v>96</v>
       </c>
@@ -2715,7 +2722,7 @@
       </c>
       <c r="F97" s="6"/>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A98" s="4">
         <v>97</v>
       </c>
@@ -2729,7 +2736,7 @@
       </c>
       <c r="F98" s="6"/>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A99" s="4">
         <v>98</v>
       </c>
@@ -2743,7 +2750,7 @@
       </c>
       <c r="F99" s="6"/>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A100" s="4">
         <v>99</v>
       </c>
@@ -2757,7 +2764,7 @@
       </c>
       <c r="F100" s="6"/>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A101" s="4">
         <v>100</v>
       </c>
@@ -2771,7 +2778,7 @@
       </c>
       <c r="F101" s="6"/>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A102" s="4">
         <v>101</v>
       </c>
@@ -2785,7 +2792,7 @@
       </c>
       <c r="F102" s="6"/>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A103" s="4">
         <v>102</v>
       </c>
@@ -2799,7 +2806,7 @@
       </c>
       <c r="F103" s="6"/>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A104" s="4">
         <v>103</v>
       </c>
@@ -2813,7 +2820,7 @@
       </c>
       <c r="F104" s="6"/>
     </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A105" s="4">
         <v>104</v>
       </c>
@@ -2827,7 +2834,7 @@
       </c>
       <c r="F105" s="6"/>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A106" s="4">
         <v>105</v>
       </c>
@@ -2841,7 +2848,7 @@
       </c>
       <c r="F106" s="6"/>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A107" s="4">
         <v>106</v>
       </c>
@@ -2855,7 +2862,7 @@
       </c>
       <c r="F107" s="6"/>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A108" s="4">
         <v>107</v>
       </c>
@@ -2869,7 +2876,7 @@
       </c>
       <c r="F108" s="6"/>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A109" s="4">
         <v>108</v>
       </c>
@@ -2883,7 +2890,7 @@
       </c>
       <c r="F109" s="6"/>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A110" s="4">
         <v>109</v>
       </c>
@@ -2897,7 +2904,7 @@
       </c>
       <c r="F110" s="6"/>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A111" s="4">
         <v>110</v>
       </c>
@@ -2911,7 +2918,7 @@
       </c>
       <c r="F111" s="6"/>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A112" s="4">
         <v>111</v>
       </c>
@@ -2925,7 +2932,7 @@
       </c>
       <c r="F112" s="6"/>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A113" s="4">
         <v>112</v>
       </c>
@@ -2939,7 +2946,7 @@
       </c>
       <c r="F113" s="6"/>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A114" s="4">
         <v>113</v>
       </c>
@@ -2953,7 +2960,7 @@
       </c>
       <c r="F114" s="6"/>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A115" s="4">
         <v>114</v>
       </c>
@@ -2967,7 +2974,7 @@
       </c>
       <c r="F115" s="6"/>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A116" s="4">
         <v>115</v>
       </c>
@@ -2981,7 +2988,7 @@
       </c>
       <c r="F116" s="6"/>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A117" s="4">
         <v>116</v>
       </c>
@@ -2995,7 +3002,7 @@
       </c>
       <c r="F117" s="6"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A118" s="4">
         <v>117</v>
       </c>
@@ -3009,7 +3016,7 @@
       </c>
       <c r="F118" s="6"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A119" s="4">
         <v>118</v>
       </c>
@@ -3023,7 +3030,7 @@
       </c>
       <c r="F119" s="6"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A120" s="4">
         <v>119</v>
       </c>
@@ -3037,7 +3044,7 @@
       </c>
       <c r="F120" s="6"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A121" s="4">
         <v>120</v>
       </c>
@@ -3051,7 +3058,7 @@
       </c>
       <c r="F121" s="6"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A122" s="4">
         <v>121</v>
       </c>
@@ -3065,7 +3072,7 @@
       </c>
       <c r="F122" s="6"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A123" s="4">
         <v>122</v>
       </c>
@@ -3079,7 +3086,7 @@
       </c>
       <c r="F123" s="6"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A124" s="4">
         <v>123</v>
       </c>
@@ -3093,7 +3100,7 @@
       </c>
       <c r="F124" s="6"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A125" s="4">
         <v>124</v>
       </c>
@@ -3107,7 +3114,7 @@
       </c>
       <c r="F125" s="6"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A126" s="4">
         <v>125</v>
       </c>
@@ -3121,7 +3128,7 @@
       </c>
       <c r="F126" s="6"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A127" s="4">
         <v>126</v>
       </c>
@@ -3135,7 +3142,7 @@
       </c>
       <c r="F127" s="6"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A128" s="4">
         <v>127</v>
       </c>
@@ -3149,7 +3156,7 @@
       </c>
       <c r="F128" s="6"/>
     </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A129" s="4">
         <v>128</v>
       </c>
@@ -3163,7 +3170,7 @@
       </c>
       <c r="F129" s="6"/>
     </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A130" s="4">
         <v>129</v>
       </c>
@@ -3177,7 +3184,7 @@
       </c>
       <c r="F130" s="6"/>
     </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A131" s="4">
         <v>130</v>
       </c>
@@ -3191,7 +3198,7 @@
       </c>
       <c r="F131" s="6"/>
     </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A132" s="4">
         <v>131</v>
       </c>
@@ -3205,7 +3212,7 @@
       </c>
       <c r="F132" s="6"/>
     </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A133" s="4">
         <v>132</v>
       </c>
@@ -3219,7 +3226,7 @@
       </c>
       <c r="F133" s="6"/>
     </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A134" s="4">
         <v>133</v>
       </c>
@@ -3233,7 +3240,7 @@
       </c>
       <c r="F134" s="6"/>
     </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A135" s="4">
         <v>134</v>
       </c>
@@ -3247,7 +3254,7 @@
       </c>
       <c r="F135" s="6"/>
     </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A136" s="4">
         <v>135</v>
       </c>
@@ -3261,7 +3268,7 @@
       </c>
       <c r="F136" s="6"/>
     </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A137" s="4">
         <v>136</v>
       </c>
@@ -3275,7 +3282,7 @@
       </c>
       <c r="F137" s="6"/>
     </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A138" s="4">
         <v>137</v>
       </c>
@@ -3289,7 +3296,7 @@
       </c>
       <c r="F138" s="6"/>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A139" s="4">
         <v>138</v>
       </c>
@@ -3303,7 +3310,7 @@
       </c>
       <c r="F139" s="6"/>
     </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A140" s="4">
         <v>139</v>
       </c>
@@ -3317,7 +3324,7 @@
       </c>
       <c r="F140" s="6"/>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A141" s="4">
         <v>140</v>
       </c>
@@ -3331,7 +3338,7 @@
       </c>
       <c r="F141" s="6"/>
     </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A142" s="4">
         <v>141</v>
       </c>
@@ -3345,7 +3352,7 @@
       </c>
       <c r="F142" s="6"/>
     </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A143" s="4">
         <v>142</v>
       </c>
@@ -3359,7 +3366,7 @@
       </c>
       <c r="F143" s="6"/>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A144" s="4">
         <v>143</v>
       </c>
@@ -3373,7 +3380,7 @@
       </c>
       <c r="F144" s="6"/>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A145" s="4">
         <v>144</v>
       </c>
@@ -3387,7 +3394,7 @@
       </c>
       <c r="F145" s="6"/>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A146" s="4">
         <v>145</v>
       </c>
@@ -3401,7 +3408,7 @@
       </c>
       <c r="F146" s="6"/>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A147" s="4">
         <v>146</v>
       </c>
@@ -3415,7 +3422,7 @@
       </c>
       <c r="F147" s="6"/>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A148" s="4">
         <v>147</v>
       </c>
@@ -3429,7 +3436,7 @@
       </c>
       <c r="F148" s="6"/>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A149" s="4">
         <v>148</v>
       </c>
@@ -3443,7 +3450,7 @@
       </c>
       <c r="F149" s="6"/>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A150" s="4">
         <v>149</v>
       </c>
@@ -3457,7 +3464,7 @@
       </c>
       <c r="F150" s="6"/>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A151" s="4">
         <v>150</v>
       </c>
@@ -3471,7 +3478,7 @@
       </c>
       <c r="F151" s="6"/>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A152" s="4">
         <v>151</v>
       </c>
@@ -3485,7 +3492,7 @@
       </c>
       <c r="F152" s="6"/>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A153" s="4">
         <v>152</v>
       </c>
@@ -3499,7 +3506,7 @@
       </c>
       <c r="F153" s="6"/>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A154" s="4">
         <v>153</v>
       </c>
@@ -3513,7 +3520,7 @@
       </c>
       <c r="F154" s="6"/>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A155" s="4">
         <v>154</v>
       </c>
@@ -3527,7 +3534,7 @@
       </c>
       <c r="F155" s="6"/>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A156" s="4">
         <v>155</v>
       </c>
@@ -3541,7 +3548,7 @@
       </c>
       <c r="F156" s="6"/>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A157" s="4">
         <v>156</v>
       </c>
@@ -3555,7 +3562,7 @@
       </c>
       <c r="F157" s="6"/>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A158" s="4">
         <v>157</v>
       </c>
@@ -3569,7 +3576,7 @@
       </c>
       <c r="F158" s="6"/>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A159" s="4">
         <v>158</v>
       </c>
@@ -3583,7 +3590,7 @@
       </c>
       <c r="F159" s="6"/>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A160" s="4">
         <v>159</v>
       </c>
@@ -3597,7 +3604,7 @@
       </c>
       <c r="F160" s="6"/>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A161" s="4">
         <v>160</v>
       </c>
@@ -3611,7 +3618,7 @@
       </c>
       <c r="F161" s="6"/>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A162" s="4">
         <v>161</v>
       </c>
@@ -3625,7 +3632,7 @@
       </c>
       <c r="F162" s="6"/>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A163" s="4">
         <v>162</v>
       </c>
@@ -3639,7 +3646,7 @@
       </c>
       <c r="F163" s="6"/>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A164" s="4">
         <v>163</v>
       </c>
@@ -3653,7 +3660,7 @@
       </c>
       <c r="F164" s="6"/>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A165" s="4">
         <v>164</v>
       </c>
@@ -3667,7 +3674,7 @@
       </c>
       <c r="F165" s="6"/>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A166" s="4">
         <v>165</v>
       </c>
@@ -3681,7 +3688,7 @@
       </c>
       <c r="F166" s="6"/>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A167" s="4">
         <v>166</v>
       </c>
@@ -3695,7 +3702,7 @@
       </c>
       <c r="F167" s="6"/>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A168" s="4">
         <v>167</v>
       </c>
@@ -3709,7 +3716,7 @@
       </c>
       <c r="F168" s="6"/>
     </row>
-    <row r="169" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A169" s="4">
         <v>168</v>
       </c>
@@ -3723,7 +3730,7 @@
       </c>
       <c r="F169" s="6"/>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A170" s="4">
         <v>169</v>
       </c>
@@ -3737,7 +3744,7 @@
       </c>
       <c r="F170" s="6"/>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A171" s="4">
         <v>170</v>
       </c>
@@ -3751,7 +3758,7 @@
       </c>
       <c r="F171" s="6"/>
     </row>
-    <row r="172" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A172" s="4">
         <v>171</v>
       </c>
@@ -3775,11 +3782,11 @@
       </c>
       <c r="D173" s="5"/>
       <c r="E173" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F173" s="6"/>
     </row>
-    <row r="174" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A174" s="4">
         <v>173</v>
       </c>
@@ -3793,7 +3800,7 @@
       </c>
       <c r="F174" s="6"/>
     </row>
-    <row r="175" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A175" s="4">
         <v>174</v>
       </c>
@@ -3807,7 +3814,7 @@
       </c>
       <c r="F175" s="6"/>
     </row>
-    <row r="176" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A176" s="4">
         <v>175</v>
       </c>
@@ -3821,7 +3828,7 @@
       </c>
       <c r="F176" s="6"/>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A177" s="4">
         <v>176</v>
       </c>
@@ -3835,7 +3842,7 @@
       </c>
       <c r="F177" s="6"/>
     </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A178" s="4">
         <v>177</v>
       </c>
@@ -3901,11 +3908,11 @@
       </c>
       <c r="D182" s="5"/>
       <c r="E182" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F182" s="6"/>
     </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A183" s="4">
         <v>182</v>
       </c>
@@ -3919,7 +3926,7 @@
       </c>
       <c r="F183" s="6"/>
     </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A184" s="4">
         <v>183</v>
       </c>
@@ -3957,11 +3964,11 @@
       </c>
       <c r="D186" s="5"/>
       <c r="E186" s="5" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="F186" s="6"/>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A187" s="4">
         <v>186</v>
       </c>
@@ -3977,7 +3984,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A188" s="4">
         <v>187</v>
       </c>
@@ -4005,33 +4012,33 @@
       </c>
       <c r="F189" s="6"/>
     </row>
-    <row r="190" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A190" s="4">
+    <row r="190" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="11">
         <v>189</v>
       </c>
-      <c r="B190" s="5"/>
-      <c r="C190" s="5" t="s">
+      <c r="B190" s="8"/>
+      <c r="C190" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="D190" s="5"/>
-      <c r="E190" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="F190" s="6"/>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A191" s="4">
+      <c r="D190" s="8"/>
+      <c r="E190" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F190" s="12"/>
+    </row>
+    <row r="191" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="11">
         <v>190</v>
       </c>
-      <c r="B191" s="5"/>
-      <c r="C191" s="5" t="s">
+      <c r="B191" s="8"/>
+      <c r="C191" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="D191" s="5"/>
-      <c r="E191" s="5" t="s">
-        <v>192</v>
-      </c>
-      <c r="F191" s="6"/>
+      <c r="D191" s="8"/>
+      <c r="E191" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F191" s="12"/>
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A192" s="4">
@@ -4090,32 +4097,32 @@
       <c r="F195" s="6"/>
     </row>
     <row r="196" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A196" s="4">
+      <c r="A196" s="11">
         <v>195</v>
       </c>
-      <c r="B196" s="5"/>
-      <c r="C196" s="11" t="s">
+      <c r="B196" s="8"/>
+      <c r="C196" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="D196" s="11"/>
-      <c r="E196" s="11" t="s">
+      <c r="D196" s="8"/>
+      <c r="E196" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="F196" s="6"/>
+      <c r="F196" s="12"/>
     </row>
     <row r="197" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A197" s="4">
+      <c r="A197" s="11">
         <v>196</v>
       </c>
-      <c r="B197" s="5"/>
-      <c r="C197" s="11" t="s">
+      <c r="B197" s="8"/>
+      <c r="C197" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="D197" s="11"/>
-      <c r="E197" s="11" t="s">
+      <c r="D197" s="8"/>
+      <c r="E197" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="F197" s="6"/>
+      <c r="F197" s="12"/>
     </row>
     <row r="198" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A198" s="4">
@@ -4145,7 +4152,7 @@
       </c>
       <c r="F199" s="6"/>
     </row>
-    <row r="200" spans="1:6" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="200" spans="1:6" ht="28.5" hidden="1" x14ac:dyDescent="0.45">
       <c r="A200" s="4"/>
       <c r="B200" s="5"/>
       <c r="C200" s="7" t="s">
@@ -4157,7 +4164,7 @@
       </c>
       <c r="F200" s="6"/>
     </row>
-    <row r="201" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A201" s="4">
         <v>199</v>
       </c>
@@ -4171,7 +4178,7 @@
       </c>
       <c r="F201" s="6"/>
     </row>
-    <row r="202" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A202" s="4">
         <v>200</v>
       </c>
@@ -4185,7 +4192,7 @@
       </c>
       <c r="F202" s="6"/>
     </row>
-    <row r="203" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A203" s="4">
         <v>201</v>
       </c>
@@ -4199,7 +4206,7 @@
       </c>
       <c r="F203" s="6"/>
     </row>
-    <row r="204" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A204" s="4">
         <v>202</v>
       </c>
@@ -4213,7 +4220,7 @@
       </c>
       <c r="F204" s="6"/>
     </row>
-    <row r="205" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A205" s="4">
         <v>203</v>
       </c>
@@ -4227,7 +4234,7 @@
       </c>
       <c r="F205" s="6"/>
     </row>
-    <row r="206" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A206" s="4">
         <v>204</v>
       </c>
@@ -4241,7 +4248,7 @@
       </c>
       <c r="F206" s="6"/>
     </row>
-    <row r="207" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A207" s="4">
         <v>205</v>
       </c>
@@ -4255,7 +4262,7 @@
       </c>
       <c r="F207" s="6"/>
     </row>
-    <row r="208" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A208" s="4">
         <v>206</v>
       </c>
@@ -4269,7 +4276,7 @@
       </c>
       <c r="F208" s="6"/>
     </row>
-    <row r="209" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A209" s="4">
         <v>207</v>
       </c>
@@ -4283,7 +4290,7 @@
       </c>
       <c r="F209" s="6"/>
     </row>
-    <row r="210" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A210" s="4">
         <v>208</v>
       </c>
@@ -4297,7 +4304,7 @@
       </c>
       <c r="F210" s="6"/>
     </row>
-    <row r="211" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A211" s="4">
         <v>209</v>
       </c>
@@ -4311,7 +4318,7 @@
       </c>
       <c r="F211" s="6"/>
     </row>
-    <row r="212" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A212" s="4">
         <v>210</v>
       </c>
@@ -4326,34 +4333,34 @@
       <c r="F212" s="6"/>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A213" s="4">
+      <c r="A213" s="11">
         <v>211</v>
       </c>
-      <c r="B213" s="5"/>
-      <c r="C213" s="11" t="s">
+      <c r="B213" s="8"/>
+      <c r="C213" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="D213" s="11"/>
-      <c r="E213" s="11" t="s">
+      <c r="D213" s="8"/>
+      <c r="E213" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="F213" s="6"/>
+      <c r="F213" s="12"/>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A214" s="4">
+      <c r="A214" s="11">
         <v>212</v>
       </c>
-      <c r="B214" s="5"/>
-      <c r="C214" s="12" t="s">
+      <c r="B214" s="8"/>
+      <c r="C214" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="D214" s="11"/>
-      <c r="E214" s="11" t="s">
+      <c r="D214" s="8"/>
+      <c r="E214" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="F214" s="6"/>
-    </row>
-    <row r="215" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="F214" s="12"/>
+    </row>
+    <row r="215" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A215" s="4">
         <v>213</v>
       </c>
@@ -4367,7 +4374,7 @@
       </c>
       <c r="F215" s="6"/>
     </row>
-    <row r="216" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A216" s="4">
         <v>214</v>
       </c>
@@ -4381,7 +4388,7 @@
       </c>
       <c r="F216" s="6"/>
     </row>
-    <row r="217" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A217" s="4">
         <v>215</v>
       </c>
@@ -4395,7 +4402,7 @@
       </c>
       <c r="F217" s="6"/>
     </row>
-    <row r="218" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:6" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A218" s="4">
         <v>216</v>
       </c>
@@ -4409,7 +4416,7 @@
       </c>
       <c r="F218" s="6"/>
     </row>
-    <row r="219" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A219" s="4">
         <v>217</v>
       </c>
@@ -4423,7 +4430,7 @@
       </c>
       <c r="F219" s="6"/>
     </row>
-    <row r="220" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A220" s="4">
         <v>218</v>
       </c>
@@ -4437,7 +4444,7 @@
       </c>
       <c r="F220" s="6"/>
     </row>
-    <row r="221" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A221" s="4">
         <v>219</v>
       </c>
@@ -4466,48 +4473,48 @@
       <c r="F222" s="6"/>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A223" s="4">
+      <c r="A223" s="11">
         <v>221</v>
       </c>
-      <c r="B223" s="5"/>
-      <c r="C223" s="11" t="s">
+      <c r="B223" s="8"/>
+      <c r="C223" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="D223" s="11"/>
-      <c r="E223" s="11" t="s">
+      <c r="D223" s="8"/>
+      <c r="E223" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="F223" s="6"/>
+      <c r="F223" s="12"/>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A224" s="4">
+      <c r="A224" s="11">
         <v>222</v>
       </c>
-      <c r="B224" s="5"/>
-      <c r="C224" s="11" t="s">
+      <c r="B224" s="8"/>
+      <c r="C224" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="D224" s="11"/>
-      <c r="E224" s="11" t="s">
+      <c r="D224" s="8"/>
+      <c r="E224" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="F224" s="6"/>
+      <c r="F224" s="12"/>
     </row>
     <row r="225" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A225" s="9">
+      <c r="A225" s="13">
         <v>223</v>
       </c>
       <c r="B225" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="C225" s="13" t="s">
+      <c r="C225" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="D225" s="13"/>
-      <c r="E225" s="13" t="s">
+      <c r="D225" s="10"/>
+      <c r="E225" s="10" t="s">
         <v>193</v>
       </c>
-      <c r="F225" s="8"/>
+      <c r="F225" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes for folders and namespaces
Changes for folders and namespaces
</commit_message>
<xml_diff>
--- a/Requirements/TotalItemList.xlsx
+++ b/Requirements/TotalItemList.xlsx
@@ -629,9 +629,6 @@
     <t>Purchase price tracking report</t>
   </si>
   <si>
-    <t>Stock &amp; sale rewports</t>
-  </si>
-  <si>
     <t>SKU wise</t>
   </si>
   <si>
@@ -654,6 +651,9 @@
   </si>
   <si>
     <t>Branch based DC #</t>
+  </si>
+  <si>
+    <t>Stock &amp; sale reports</t>
   </si>
 </sst>
 </file>
@@ -1344,7 +1344,7 @@
   <dimension ref="A1:F225"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D185" sqref="D185"/>
+      <selection activeCell="D189" sqref="D189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1812,19 +1812,19 @@
       </c>
       <c r="F32" s="6"/>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="11">
         <v>32</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5" t="s">
+      <c r="B33" s="8"/>
+      <c r="C33" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="F33" s="6"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F33" s="12"/>
     </row>
     <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
@@ -1882,19 +1882,19 @@
       </c>
       <c r="F37" s="6"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+    <row r="38" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="11">
         <v>37</v>
       </c>
-      <c r="B38" s="5"/>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5" t="s">
+      <c r="B38" s="8"/>
+      <c r="C38" s="8"/>
+      <c r="D38" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E38" s="5" t="s">
-        <v>193</v>
-      </c>
-      <c r="F38" s="6"/>
+      <c r="E38" s="8" t="s">
+        <v>192</v>
+      </c>
+      <c r="F38" s="12"/>
     </row>
     <row r="39" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
@@ -4046,7 +4046,7 @@
       </c>
       <c r="B192" s="5"/>
       <c r="C192" s="5" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="D192" s="5"/>
       <c r="E192" s="5" t="s">
@@ -4061,7 +4061,7 @@
       <c r="B193" s="5"/>
       <c r="C193" s="5"/>
       <c r="D193" s="5" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E193" s="5" t="s">
         <v>193</v>
@@ -4075,7 +4075,7 @@
       <c r="B194" s="5"/>
       <c r="C194" s="5"/>
       <c r="D194" s="5" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E194" s="5" t="s">
         <v>193</v>
@@ -4089,14 +4089,14 @@
       <c r="B195" s="5"/>
       <c r="C195" s="5"/>
       <c r="D195" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E195" s="5" t="s">
         <v>193</v>
       </c>
       <c r="F195" s="6"/>
     </row>
-    <row r="196" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A196" s="11">
         <v>195</v>
       </c>
@@ -4106,21 +4106,21 @@
       </c>
       <c r="D196" s="8"/>
       <c r="E196" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F196" s="12"/>
     </row>
-    <row r="197" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A197" s="11">
         <v>196</v>
       </c>
       <c r="B197" s="8"/>
       <c r="C197" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D197" s="8"/>
       <c r="E197" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F197" s="12"/>
     </row>
@@ -4130,7 +4130,7 @@
       </c>
       <c r="B198" s="5"/>
       <c r="C198" s="5" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D198" s="5"/>
       <c r="E198" s="5" t="s">
@@ -4144,7 +4144,7 @@
       </c>
       <c r="B199" s="5"/>
       <c r="C199" s="5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D199" s="5"/>
       <c r="E199" s="5" t="s">
@@ -4332,7 +4332,7 @@
       </c>
       <c r="F212" s="6"/>
     </row>
-    <row r="213" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A213" s="11">
         <v>211</v>
       </c>
@@ -4342,11 +4342,11 @@
       </c>
       <c r="D213" s="8"/>
       <c r="E213" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F213" s="12"/>
     </row>
-    <row r="214" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A214" s="11">
         <v>212</v>
       </c>
@@ -4356,7 +4356,7 @@
       </c>
       <c r="D214" s="8"/>
       <c r="E214" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F214" s="12"/>
     </row>
@@ -4472,7 +4472,7 @@
       </c>
       <c r="F222" s="6"/>
     </row>
-    <row r="223" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A223" s="11">
         <v>221</v>
       </c>
@@ -4482,25 +4482,25 @@
       </c>
       <c r="D223" s="8"/>
       <c r="E223" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F223" s="12"/>
     </row>
-    <row r="224" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A224" s="11">
         <v>222</v>
       </c>
       <c r="B224" s="8"/>
       <c r="C224" s="8" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D224" s="8"/>
       <c r="E224" s="8" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F224" s="12"/>
     </row>
-    <row r="225" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:6" hidden="1" x14ac:dyDescent="0.25">
       <c r="A225" s="13">
         <v>223</v>
       </c>
@@ -4508,11 +4508,11 @@
         <v>3</v>
       </c>
       <c r="C225" s="10" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D225" s="10"/>
       <c r="E225" s="10" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="F225" s="14"/>
     </row>

</xml_diff>